<commit_message>
Fixed the overall total calculation to only sum up the net profit of each sheet.
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -16,12 +16,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -66,8 +67,14 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -77,6 +84,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -178,6 +191,30 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -544,7 +581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1586,13 +1623,375 @@
       </c>
     </row>
     <row r="57">
-      <c r="B57" s="17" t="inlineStr">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>FY23-24 Q1 St. Gallen Summer '23</t>
+        </is>
+      </c>
+      <c r="B57" s="2" t="n"/>
+      <c r="C57" s="2" t="n"/>
+      <c r="D57" s="2" t="n"/>
+      <c r="E57" s="2" t="n"/>
+      <c r="F57" s="2" t="n"/>
+      <c r="G57" s="2" t="n"/>
+      <c r="H57" s="2" t="n"/>
+      <c r="I57" s="2" t="n"/>
+      <c r="J57" s="2" t="n"/>
+      <c r="K57" s="2" t="n"/>
+      <c r="L57" s="2" t="n"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="inlineStr">
+        <is>
+          <t>Summary of Key Financial Metrics for the LDI Financial Forecast Spreadsheet</t>
+        </is>
+      </c>
+      <c r="B58" s="4" t="n"/>
+      <c r="C58" s="4" t="n"/>
+      <c r="D58" s="4" t="n"/>
+      <c r="E58" s="4" t="n"/>
+      <c r="F58" s="4" t="n"/>
+      <c r="G58" s="4" t="n"/>
+      <c r="H58" s="4" t="n"/>
+      <c r="I58" s="4" t="n"/>
+      <c r="J58" s="4" t="n"/>
+      <c r="K58" s="4" t="n"/>
+      <c r="L58" s="4" t="n"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="5" t="inlineStr">
+        <is>
+          <t># of Students</t>
+        </is>
+      </c>
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>Price ($)/Student</t>
+        </is>
+      </c>
+      <c r="D59" s="5" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="E59" s="5" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="F59" s="5" t="inlineStr">
+        <is>
+          <t>Gross Profit</t>
+        </is>
+      </c>
+      <c r="G59" s="5" t="inlineStr">
+        <is>
+          <t>LDI Overhead</t>
+        </is>
+      </c>
+      <c r="H59" s="5" t="inlineStr">
+        <is>
+          <t>EBITA</t>
+        </is>
+      </c>
+      <c r="I59" s="5" t="inlineStr">
+        <is>
+          <t>SIA</t>
+        </is>
+      </c>
+      <c r="J59" s="5" t="inlineStr">
+        <is>
+          <t>G&amp;A</t>
+        </is>
+      </c>
+      <c r="K59" s="5" t="inlineStr">
+        <is>
+          <t>Net Profit</t>
+        </is>
+      </c>
+      <c r="L59" s="5" t="inlineStr">
+        <is>
+          <t>Margin</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="n">
+        <v>38</v>
+      </c>
+      <c r="C60" s="7" t="n">
+        <v>4407.894736842105</v>
+      </c>
+      <c r="D60" s="8" t="n">
+        <v>167500</v>
+      </c>
+      <c r="E60" s="9" t="n">
+        <v>75843</v>
+      </c>
+      <c r="F60" s="8" t="n">
+        <v>91657</v>
+      </c>
+      <c r="G60" s="9" t="n">
+        <v>67000</v>
+      </c>
+      <c r="H60" s="9" t="n">
+        <v>24657</v>
+      </c>
+      <c r="I60" s="9" t="n">
+        <v>45469.963</v>
+      </c>
+      <c r="J60" s="9" t="n">
+        <v>7581.669631199999</v>
+      </c>
+      <c r="K60" s="9" t="n">
+        <v>-28394.6326312</v>
+      </c>
+      <c r="L60" s="10" t="n">
+        <v>-0.1695201948131344</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>FY23-24 Q4 UCI Radiology Summer '23</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="n"/>
+      <c r="C64" s="2" t="n"/>
+      <c r="D64" s="2" t="n"/>
+      <c r="E64" s="2" t="n"/>
+      <c r="F64" s="2" t="n"/>
+      <c r="G64" s="2" t="n"/>
+      <c r="H64" s="2" t="n"/>
+      <c r="I64" s="2" t="n"/>
+      <c r="J64" s="2" t="n"/>
+      <c r="K64" s="2" t="n"/>
+      <c r="L64" s="2" t="n"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="17" t="n"/>
+      <c r="C65" s="7" t="n"/>
+      <c r="D65" s="18" t="n"/>
+      <c r="E65" s="19" t="n"/>
+      <c r="F65" s="20" t="n"/>
+      <c r="G65" s="21" t="n"/>
+      <c r="H65" s="21" t="n"/>
+      <c r="I65" s="21" t="n"/>
+      <c r="J65" s="22" t="n"/>
+      <c r="K65" s="23" t="n"/>
+      <c r="L65" s="23" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>Summary of Key Financial Metrics for the LDI Financial Forecast Spreadsheet</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="n"/>
+      <c r="C66" s="4" t="n"/>
+      <c r="D66" s="4" t="n"/>
+      <c r="E66" s="4" t="n"/>
+      <c r="F66" s="4" t="n"/>
+      <c r="G66" s="4" t="n"/>
+      <c r="H66" s="4" t="n"/>
+      <c r="I66" s="4" t="n"/>
+      <c r="J66" s="4" t="n"/>
+      <c r="K66" s="4" t="n"/>
+      <c r="L66" s="4" t="n"/>
+    </row>
+    <row r="67">
+      <c r="B67" s="5" t="inlineStr">
+        <is>
+          <t># of Students</t>
+        </is>
+      </c>
+      <c r="C67" s="6" t="inlineStr">
+        <is>
+          <t>Price ($)/Student</t>
+        </is>
+      </c>
+      <c r="D67" s="5" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="E67" s="5" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="F67" s="5" t="inlineStr">
+        <is>
+          <t>Gross Profit</t>
+        </is>
+      </c>
+      <c r="G67" s="5" t="inlineStr">
+        <is>
+          <t>LDI Overhead</t>
+        </is>
+      </c>
+      <c r="H67" s="5" t="inlineStr">
+        <is>
+          <t>EBITA</t>
+        </is>
+      </c>
+      <c r="I67" s="5" t="inlineStr">
+        <is>
+          <t>SIA</t>
+        </is>
+      </c>
+      <c r="J67" s="5" t="inlineStr">
+        <is>
+          <t>G&amp;A</t>
+        </is>
+      </c>
+      <c r="K67" s="5" t="inlineStr">
+        <is>
+          <t>Net Profit</t>
+        </is>
+      </c>
+      <c r="L67" s="5" t="inlineStr">
+        <is>
+          <t>Margin</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>FY23-24 Q1 Yonsei Summer '23</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="n"/>
+      <c r="C71" s="2" t="n"/>
+      <c r="D71" s="2" t="n"/>
+      <c r="E71" s="2" t="n"/>
+      <c r="F71" s="2" t="n"/>
+      <c r="G71" s="2" t="n"/>
+      <c r="H71" s="2" t="n"/>
+      <c r="I71" s="2" t="n"/>
+      <c r="J71" s="2" t="n"/>
+      <c r="K71" s="2" t="n"/>
+      <c r="L71" s="2" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="4" t="inlineStr">
+        <is>
+          <t>Summary of Key Financial Metrics for the LDI Financial Forecast Spreadsheet</t>
+        </is>
+      </c>
+      <c r="B72" s="4" t="n"/>
+      <c r="C72" s="4" t="n"/>
+      <c r="D72" s="4" t="n"/>
+      <c r="E72" s="4" t="n"/>
+      <c r="F72" s="4" t="n"/>
+      <c r="G72" s="4" t="n"/>
+      <c r="H72" s="4" t="n"/>
+      <c r="I72" s="4" t="n"/>
+      <c r="J72" s="4" t="n"/>
+      <c r="K72" s="4" t="n"/>
+      <c r="L72" s="4" t="n"/>
+    </row>
+    <row r="73">
+      <c r="B73" s="5" t="inlineStr">
+        <is>
+          <t># of Students</t>
+        </is>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>Price ($)/Student</t>
+        </is>
+      </c>
+      <c r="D73" s="5" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="E73" s="5" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="F73" s="5" t="inlineStr">
+        <is>
+          <t>Gross Profit</t>
+        </is>
+      </c>
+      <c r="G73" s="5" t="inlineStr">
+        <is>
+          <t>LDI Overhead</t>
+        </is>
+      </c>
+      <c r="H73" s="5" t="inlineStr">
+        <is>
+          <t>EBITA</t>
+        </is>
+      </c>
+      <c r="I73" s="5" t="inlineStr">
+        <is>
+          <t>SIA</t>
+        </is>
+      </c>
+      <c r="J73" s="5" t="inlineStr">
+        <is>
+          <t>G&amp;A</t>
+        </is>
+      </c>
+      <c r="K73" s="5" t="inlineStr">
+        <is>
+          <t>Net Profit</t>
+        </is>
+      </c>
+      <c r="L73" s="5" t="inlineStr">
+        <is>
+          <t>Margin</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="n">
+        <v>20</v>
+      </c>
+      <c r="C74" s="24" t="n">
+        <v>5500</v>
+      </c>
+      <c r="D74" s="25" t="n">
+        <v>105000</v>
+      </c>
+      <c r="E74" s="26" t="n">
+        <v>32544.5</v>
+      </c>
+      <c r="F74" s="26" t="n">
+        <v>77455.5</v>
+      </c>
+      <c r="G74" s="26" t="n">
+        <v>44000</v>
+      </c>
+      <c r="H74" s="26" t="n">
+        <v>39755.5</v>
+      </c>
+      <c r="I74" s="26" t="n">
+        <v>23953.3745</v>
+      </c>
+      <c r="J74" s="26" t="n">
+        <v>3993.9898788</v>
+      </c>
+      <c r="K74" s="9" t="n">
+        <v>5508.135621199998</v>
+      </c>
+      <c r="L74" s="10" t="n">
+        <v>0.05245843448761903</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" s="27" t="inlineStr">
         <is>
           <t>Overall Total:</t>
         </is>
       </c>
-      <c r="C57" s="9" t="n">
-        <v>3297885.8</v>
+      <c r="C78" s="9" t="n">
+        <v>120177.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>